<commit_message>
cleanup GA+MIL mess + addded MIL stands
</commit_message>
<xml_diff>
--- a/api/data/parking_coords.xlsx
+++ b/api/data/parking_coords.xlsx
@@ -5,27 +5,36 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEV\beluxvacc\belux-gate-manager-api\api\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\belux\belux-gate-manager-api\api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A925E3C0-EAA8-4897-B7E5-A98684E3A9AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF19E24-6EC3-4CFA-9B71-68026515DA5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A18B69D9-28ED-47D3-8556-C314F1DB8CFD}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A18B69D9-28ED-47D3-8556-C314F1DB8CFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="425">
   <si>
     <t>505335.23N</t>
   </si>
@@ -2346,24 +2355,6 @@
     <t>apron-60</t>
   </si>
   <si>
-    <t>MIL1</t>
-  </si>
-  <si>
-    <t>MIL2</t>
-  </si>
-  <si>
-    <t>MIL3</t>
-  </si>
-  <si>
-    <t>MIL5</t>
-  </si>
-  <si>
-    <t>MIL7</t>
-  </si>
-  <si>
-    <t>MIL9</t>
-  </si>
-  <si>
     <t>MIL11</t>
   </si>
   <si>
@@ -2377,6 +2368,57 @@
   </si>
   <si>
     <t>apron-MIL</t>
+  </si>
+  <si>
+    <t>MIL01</t>
+  </si>
+  <si>
+    <t>MIL02</t>
+  </si>
+  <si>
+    <t>MIL03</t>
+  </si>
+  <si>
+    <t>MIL05</t>
+  </si>
+  <si>
+    <t>MIL07</t>
+  </si>
+  <si>
+    <t>MIL09</t>
+  </si>
+  <si>
+    <t>GA10</t>
+  </si>
+  <si>
+    <t>GA01</t>
+  </si>
+  <si>
+    <t>GA02</t>
+  </si>
+  <si>
+    <t>GA03</t>
+  </si>
+  <si>
+    <t>GA04</t>
+  </si>
+  <si>
+    <t>GA05</t>
+  </si>
+  <si>
+    <t>GA06</t>
+  </si>
+  <si>
+    <t>GA07</t>
+  </si>
+  <si>
+    <t>GA08</t>
+  </si>
+  <si>
+    <t>GA09</t>
+  </si>
+  <si>
+    <t>apron-GA</t>
   </si>
 </sst>
 </file>
@@ -2812,29 +2854,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A74C131-8C0C-4CF6-B99D-A6421F63E231}">
-  <dimension ref="A1:N187"/>
+  <dimension ref="A1:N197"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J177" sqref="J177"/>
+    <sheetView tabSelected="1" topLeftCell="A164" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C194" sqref="C194"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5546875" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>377</v>
       </c>
@@ -2878,7 +2920,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>391</v>
       </c>
@@ -2892,12 +2934,12 @@
         <v>245</v>
       </c>
       <c r="E2" t="str">
-        <f>SUBSTITUTE( SUBSTITUTE(C2,"N",""),".",",")</f>
-        <v xml:space="preserve">505404,61 </v>
+        <f>SUBSTITUTE( SUBSTITUTE(C2,"N",""),",",".")</f>
+        <v xml:space="preserve">505404.61 </v>
       </c>
       <c r="F2" t="str">
-        <f>SUBSTITUTE( SUBSTITUTE(D2,"E",""),".",",")</f>
-        <v xml:space="preserve">0042834,44 </v>
+        <f>SUBSTITUTE( SUBSTITUTE(D2,"E",""),",",".")</f>
+        <v xml:space="preserve">0042834.44 </v>
       </c>
       <c r="G2">
         <f t="shared" ref="G2:G33" si="0">_xlfn.FLOOR.MATH(E2/10000)</f>
@@ -2932,7 +2974,7 @@
         <v>4.476233333333334</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>391</v>
       </c>
@@ -2946,12 +2988,12 @@
         <v>246</v>
       </c>
       <c r="E3" t="str">
-        <f t="shared" ref="E3:E66" si="3">SUBSTITUTE( SUBSTITUTE(C3,"N",""),".",",")</f>
-        <v xml:space="preserve">505405,36 </v>
+        <f t="shared" ref="E3:E66" si="3">SUBSTITUTE( SUBSTITUTE(C3,"N",""),",",".")</f>
+        <v xml:space="preserve">505405.36 </v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F66" si="4">SUBSTITUTE( SUBSTITUTE(D3,"E",""),".",",")</f>
-        <v xml:space="preserve">0042837,07 </v>
+        <f t="shared" ref="F3:F66" si="4">SUBSTITUTE( SUBSTITUTE(D3,"E",""),",",".")</f>
+        <v xml:space="preserve">0042837.07 </v>
       </c>
       <c r="G3">
         <f t="shared" si="0"/>
@@ -2986,7 +3028,7 @@
         <v>4.4769638888888892</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>391</v>
       </c>
@@ -3001,11 +3043,11 @@
       </c>
       <c r="E4" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505406,03 </v>
+        <v xml:space="preserve">505406.03 </v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042839,40 </v>
+        <v xml:space="preserve">0042839.40 </v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
@@ -3040,7 +3082,7 @@
         <v>4.4776111111111119</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>391</v>
       </c>
@@ -3055,11 +3097,11 @@
       </c>
       <c r="E5" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505406,70 </v>
+        <v xml:space="preserve">505406.70 </v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042841,73 </v>
+        <v xml:space="preserve">0042841.73 </v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
@@ -3094,7 +3136,7 @@
         <v>4.4782583333333346</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>391</v>
       </c>
@@ -3109,11 +3151,11 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505407,38 </v>
+        <v xml:space="preserve">505407.38 </v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042844,06 </v>
+        <v xml:space="preserve">0042844.06 </v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
@@ -3148,7 +3190,7 @@
         <v>4.4789055555555546</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>391</v>
       </c>
@@ -3163,11 +3205,11 @@
       </c>
       <c r="E7" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505408,05 </v>
+        <v xml:space="preserve">505408.05 </v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042846,38 </v>
+        <v xml:space="preserve">0042846.38 </v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
@@ -3202,7 +3244,7 @@
         <v>4.4795499999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>392</v>
       </c>
@@ -3217,11 +3259,11 @@
       </c>
       <c r="E8" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505408,54 </v>
+        <v xml:space="preserve">505408.54 </v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042849,54 </v>
+        <v xml:space="preserve">0042849.54 </v>
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
@@ -3256,7 +3298,7 @@
         <v>4.4804277777777779</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>392</v>
       </c>
@@ -3271,11 +3313,11 @@
       </c>
       <c r="E9" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505409,12 </v>
+        <v xml:space="preserve">505409.12 </v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042851,55 </v>
+        <v xml:space="preserve">0042851.55 </v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
@@ -3310,7 +3352,7 @@
         <v>4.480986111111112</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>392</v>
       </c>
@@ -3325,11 +3367,11 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505409,70 </v>
+        <v xml:space="preserve">505409.70 </v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042853,56 </v>
+        <v xml:space="preserve">0042853.56 </v>
       </c>
       <c r="G10">
         <f t="shared" si="0"/>
@@ -3364,7 +3406,7 @@
         <v>4.4815444444444443</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>392</v>
       </c>
@@ -3379,11 +3421,11 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505410,29 </v>
+        <v xml:space="preserve">505410.29 </v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042855,57 </v>
+        <v xml:space="preserve">0042855.57 </v>
       </c>
       <c r="G11">
         <f t="shared" si="0"/>
@@ -3418,7 +3460,7 @@
         <v>4.4821027777777775</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>392</v>
       </c>
@@ -3433,11 +3475,11 @@
       </c>
       <c r="E12" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505410,84 </v>
+        <v xml:space="preserve">505410.84 </v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042857,61 </v>
+        <v xml:space="preserve">0042857.61 </v>
       </c>
       <c r="G12">
         <f t="shared" si="0"/>
@@ -3472,7 +3514,7 @@
         <v>4.4826694444444444</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>392</v>
       </c>
@@ -3487,11 +3529,11 @@
       </c>
       <c r="E13" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505411,42 </v>
+        <v xml:space="preserve">505411.42 </v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042859,61 </v>
+        <v xml:space="preserve">0042859.61 </v>
       </c>
       <c r="G13">
         <f t="shared" si="0"/>
@@ -3526,7 +3568,7 @@
         <v>4.483225</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>392</v>
       </c>
@@ -3541,11 +3583,11 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505411,99 </v>
+        <v xml:space="preserve">505411.99 </v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042901,63 </v>
+        <v xml:space="preserve">0042901.63 </v>
       </c>
       <c r="G14">
         <f t="shared" si="0"/>
@@ -3580,7 +3622,7 @@
         <v>4.4837861111111108</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>392</v>
       </c>
@@ -3595,11 +3637,11 @@
       </c>
       <c r="E15" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505412,57 </v>
+        <v xml:space="preserve">505412.57 </v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042903,64 </v>
+        <v xml:space="preserve">0042903.64 </v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
@@ -3634,7 +3676,7 @@
         <v>4.484344444444444</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>392</v>
       </c>
@@ -3649,11 +3691,11 @@
       </c>
       <c r="E16" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505413,16 </v>
+        <v xml:space="preserve">505413.16 </v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042905,65 </v>
+        <v xml:space="preserve">0042905.65 </v>
       </c>
       <c r="G16">
         <f t="shared" si="0"/>
@@ -3688,7 +3730,7 @@
         <v>4.4849027777777781</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>392</v>
       </c>
@@ -3703,11 +3745,11 @@
       </c>
       <c r="E17" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505413,74 </v>
+        <v xml:space="preserve">505413.74 </v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042907,66 </v>
+        <v xml:space="preserve">0042907.66 </v>
       </c>
       <c r="G17">
         <f t="shared" si="0"/>
@@ -3742,7 +3784,7 @@
         <v>4.4854611111111122</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>392</v>
       </c>
@@ -3757,11 +3799,11 @@
       </c>
       <c r="E18" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505414,32 </v>
+        <v xml:space="preserve">505414.32 </v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042909,68 </v>
+        <v xml:space="preserve">0042909.68 </v>
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
@@ -3796,7 +3838,7 @@
         <v>4.4860222222222221</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>392</v>
       </c>
@@ -3811,11 +3853,11 @@
       </c>
       <c r="E19" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505415,19 </v>
+        <v xml:space="preserve">505415.19 </v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042912,56 </v>
+        <v xml:space="preserve">0042912.56 </v>
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
@@ -3850,7 +3892,7 @@
         <v>4.486822222222222</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>392</v>
       </c>
@@ -3865,11 +3907,11 @@
       </c>
       <c r="E20" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505415,71 </v>
+        <v xml:space="preserve">505415.71 </v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042914,61 </v>
+        <v xml:space="preserve">0042914.61 </v>
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
@@ -3904,7 +3946,7 @@
         <v>4.4873916666666664</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>392</v>
       </c>
@@ -3919,11 +3961,11 @@
       </c>
       <c r="E21" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505416,32 </v>
+        <v xml:space="preserve">505416.32 </v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042916,60 </v>
+        <v xml:space="preserve">0042916.60 </v>
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
@@ -3958,7 +4000,7 @@
         <v>4.4879444444444445</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>392</v>
       </c>
@@ -3973,11 +4015,11 @@
       </c>
       <c r="E22" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505416,87 </v>
+        <v xml:space="preserve">505416.87 </v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042918,63 </v>
+        <v xml:space="preserve">0042918.63 </v>
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
@@ -4012,7 +4054,7 @@
         <v>4.4885083333333329</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>392</v>
       </c>
@@ -4027,11 +4069,11 @@
       </c>
       <c r="E23" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505417,48 </v>
+        <v xml:space="preserve">505417.48 </v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042920,62 </v>
+        <v xml:space="preserve">0042920.62 </v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
@@ -4066,7 +4108,7 @@
         <v>4.4890611111111118</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>392</v>
       </c>
@@ -4081,11 +4123,11 @@
       </c>
       <c r="E24" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505418,03 </v>
+        <v xml:space="preserve">505418.03 </v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042922,66 </v>
+        <v xml:space="preserve">0042922.66 </v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
@@ -4120,7 +4162,7 @@
         <v>4.4896277777777787</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>392</v>
       </c>
@@ -4135,11 +4177,11 @@
       </c>
       <c r="E25" t="str">
         <f t="shared" si="3"/>
-        <v>505418,41</v>
+        <v>505418.41</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="4"/>
-        <v>0042924,88</v>
+        <v>0042924.88</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
@@ -4174,7 +4216,7 @@
         <v>4.4902444444444436</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>393</v>
       </c>
@@ -4189,11 +4231,11 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505407,32 </v>
+        <v xml:space="preserve">505407.32 </v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042858,46 </v>
+        <v xml:space="preserve">0042858.46 </v>
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
@@ -4228,7 +4270,7 @@
         <v>4.482905555555555</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>393</v>
       </c>
@@ -4243,11 +4285,11 @@
       </c>
       <c r="E27" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505408,04 </v>
+        <v xml:space="preserve">505408.04 </v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042859,55 </v>
+        <v xml:space="preserve">0042859.55 </v>
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
@@ -4282,7 +4324,7 @@
         <v>4.4832083333333346</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>393</v>
       </c>
@@ -4297,11 +4339,11 @@
       </c>
       <c r="E28" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505408,16 </v>
+        <v xml:space="preserve">505408.16 </v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042900,28 </v>
+        <v xml:space="preserve">0042900.28 </v>
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
@@ -4336,7 +4378,7 @@
         <v>4.4834111111111108</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>393</v>
       </c>
@@ -4351,11 +4393,11 @@
       </c>
       <c r="E29" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505408,74 </v>
+        <v xml:space="preserve">505408.74 </v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042902,29 </v>
+        <v xml:space="preserve">0042902.29 </v>
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
@@ -4390,7 +4432,7 @@
         <v>4.4839694444444449</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>393</v>
       </c>
@@ -4405,11 +4447,11 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505409,12 </v>
+        <v xml:space="preserve">505409.12 </v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042903,62 </v>
+        <v xml:space="preserve">0042903.62 </v>
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
@@ -4444,7 +4486,7 @@
         <v>4.4843388888888898</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>393</v>
       </c>
@@ -4459,11 +4501,11 @@
       </c>
       <c r="E31" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505409,32 </v>
+        <v xml:space="preserve">505409.32 </v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042904,31 </v>
+        <v xml:space="preserve">0042904.31 </v>
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
@@ -4498,7 +4540,7 @@
         <v>4.4845305555555548</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>393</v>
       </c>
@@ -4513,11 +4555,11 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505409,90 </v>
+        <v xml:space="preserve">505409.90 </v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042906,32 </v>
+        <v xml:space="preserve">0042906.32 </v>
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
@@ -4552,7 +4594,7 @@
         <v>4.4850888888888889</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>393</v>
       </c>
@@ -4567,11 +4609,11 @@
       </c>
       <c r="E33" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505410,29 </v>
+        <v xml:space="preserve">505410.29 </v>
       </c>
       <c r="F33" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042907,64 </v>
+        <v xml:space="preserve">0042907.64 </v>
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
@@ -4606,7 +4648,7 @@
         <v>4.4854555555555553</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>393</v>
       </c>
@@ -4621,11 +4663,11 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505410,48 </v>
+        <v xml:space="preserve">505410.48 </v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042908,33 </v>
+        <v xml:space="preserve">0042908.33 </v>
       </c>
       <c r="G34">
         <f t="shared" ref="G34:G65" si="11">_xlfn.FLOOR.MATH(E34/10000)</f>
@@ -4660,7 +4702,7 @@
         <v>4.485647222222223</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>393</v>
       </c>
@@ -4675,11 +4717,11 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505411,06 </v>
+        <v xml:space="preserve">505411.06 </v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042910,34 </v>
+        <v xml:space="preserve">0042910.34 </v>
       </c>
       <c r="G35">
         <f t="shared" si="11"/>
@@ -4714,7 +4756,7 @@
         <v>4.4862055555555544</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>393</v>
       </c>
@@ -4729,11 +4771,11 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505411,45 </v>
+        <v xml:space="preserve">505411.45 </v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042911,67 </v>
+        <v xml:space="preserve">0042911.67 </v>
       </c>
       <c r="G36">
         <f t="shared" si="11"/>
@@ -4768,7 +4810,7 @@
         <v>4.4865749999999993</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>393</v>
       </c>
@@ -4783,11 +4825,11 @@
       </c>
       <c r="E37" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505411,64 </v>
+        <v xml:space="preserve">505411.64 </v>
       </c>
       <c r="F37" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042912,35 </v>
+        <v xml:space="preserve">0042912.35 </v>
       </c>
       <c r="G37">
         <f t="shared" si="11"/>
@@ -4822,7 +4864,7 @@
         <v>4.4867638888888886</v>
       </c>
     </row>
-    <row r="38" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>393</v>
       </c>
@@ -4837,11 +4879,11 @@
       </c>
       <c r="E38" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505412,05 </v>
+        <v xml:space="preserve">505412.05 </v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042914,48 </v>
+        <v xml:space="preserve">0042914.48 </v>
       </c>
       <c r="G38">
         <f t="shared" si="11"/>
@@ -4876,7 +4918,7 @@
         <v>4.4873555555555562</v>
       </c>
     </row>
-    <row r="39" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>393</v>
       </c>
@@ -4891,11 +4933,11 @@
       </c>
       <c r="E39" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505413,18 </v>
+        <v xml:space="preserve">505413.18 </v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042917,27 </v>
+        <v xml:space="preserve">0042917.27 </v>
       </c>
       <c r="G39">
         <f t="shared" si="11"/>
@@ -4930,7 +4972,7 @@
         <v>4.4881305555555544</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>393</v>
       </c>
@@ -4945,11 +4987,11 @@
       </c>
       <c r="E40" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505413,65 </v>
+        <v xml:space="preserve">505413.65 </v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042919,29 </v>
+        <v xml:space="preserve">0042919.29 </v>
       </c>
       <c r="G40">
         <f t="shared" si="11"/>
@@ -4984,7 +5026,7 @@
         <v>4.488691666666667</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>393</v>
       </c>
@@ -4999,11 +5041,11 @@
       </c>
       <c r="E41" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505414,03 </v>
+        <v xml:space="preserve">505414.03 </v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042920,60 </v>
+        <v xml:space="preserve">0042920.60 </v>
       </c>
       <c r="G41">
         <f t="shared" si="11"/>
@@ -5038,7 +5080,7 @@
         <v>4.4890555555555549</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>393</v>
       </c>
@@ -5053,11 +5095,11 @@
       </c>
       <c r="E42" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505414,22 </v>
+        <v xml:space="preserve">505414.22 </v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042921,28 </v>
+        <v xml:space="preserve">0042921.28 </v>
       </c>
       <c r="G42">
         <f t="shared" si="11"/>
@@ -5092,7 +5134,7 @@
         <v>4.4892444444444441</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>393</v>
       </c>
@@ -5107,11 +5149,11 @@
       </c>
       <c r="E43" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505414,81 </v>
+        <v xml:space="preserve">505414.81 </v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042923,30 </v>
+        <v xml:space="preserve">0042923.30 </v>
       </c>
       <c r="G43">
         <f t="shared" si="11"/>
@@ -5146,7 +5188,7 @@
         <v>4.4898055555555567</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>393</v>
       </c>
@@ -5161,11 +5203,11 @@
       </c>
       <c r="E44" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505415,32 </v>
+        <v xml:space="preserve">505415.32 </v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042925,07 </v>
+        <v xml:space="preserve">0042925.07 </v>
       </c>
       <c r="G44">
         <f t="shared" si="11"/>
@@ -5200,7 +5242,7 @@
         <v>4.4902972222222219</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>393</v>
       </c>
@@ -5215,11 +5257,11 @@
       </c>
       <c r="E45" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505415,27 </v>
+        <v xml:space="preserve">505415.27 </v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042925,39 </v>
+        <v xml:space="preserve">0042925.39 </v>
       </c>
       <c r="G45">
         <f t="shared" si="11"/>
@@ -5254,7 +5296,7 @@
         <v>4.4903861111111114</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>393</v>
       </c>
@@ -5269,11 +5311,11 @@
       </c>
       <c r="E46" t="str">
         <f t="shared" si="3"/>
-        <v>505416,04</v>
+        <v>505416.04</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="4"/>
-        <v>0042926,91</v>
+        <v>0042926.91</v>
       </c>
       <c r="G46">
         <f t="shared" si="11"/>
@@ -5308,7 +5350,7 @@
         <v>4.4908083333333346</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>394</v>
       </c>
@@ -5323,11 +5365,11 @@
       </c>
       <c r="E47" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505359,37 </v>
+        <v xml:space="preserve">505359.37 </v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042905,33 </v>
+        <v xml:space="preserve">0042905.33 </v>
       </c>
       <c r="G47">
         <f t="shared" si="11"/>
@@ -5362,7 +5404,7 @@
         <v>4.4848138888888895</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>394</v>
       </c>
@@ -5377,11 +5419,11 @@
       </c>
       <c r="E48" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505400,02 </v>
+        <v xml:space="preserve">505400.02 </v>
       </c>
       <c r="F48" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042908,41 </v>
+        <v xml:space="preserve">0042908.41 </v>
       </c>
       <c r="G48">
         <f t="shared" si="11"/>
@@ -5416,7 +5458,7 @@
         <v>4.4856694444444454</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>394</v>
       </c>
@@ -5431,11 +5473,11 @@
       </c>
       <c r="E49" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505400,10 </v>
+        <v xml:space="preserve">505400.10 </v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042907,43 </v>
+        <v xml:space="preserve">0042907.43 </v>
       </c>
       <c r="G49">
         <f t="shared" si="11"/>
@@ -5470,7 +5512,7 @@
         <v>4.4853972222222227</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>394</v>
       </c>
@@ -5485,11 +5527,11 @@
       </c>
       <c r="E50" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505400,56 </v>
+        <v xml:space="preserve">505400.56 </v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042909,38 </v>
+        <v xml:space="preserve">0042909.38 </v>
       </c>
       <c r="G50">
         <f t="shared" si="11"/>
@@ -5524,7 +5566,7 @@
         <v>4.4859388888888878</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>394</v>
       </c>
@@ -5539,11 +5581,11 @@
       </c>
       <c r="E51" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505400,99 </v>
+        <v xml:space="preserve">505400.99 </v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042911,73 </v>
+        <v xml:space="preserve">0042911.73 </v>
       </c>
       <c r="G51">
         <f t="shared" si="11"/>
@@ -5578,7 +5620,7 @@
         <v>4.4865916666666674</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>394</v>
       </c>
@@ -5593,11 +5635,11 @@
       </c>
       <c r="E52" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505401,20 </v>
+        <v xml:space="preserve">505401.20 </v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042911,22 </v>
+        <v xml:space="preserve">0042911.22 </v>
       </c>
       <c r="G52">
         <f t="shared" si="11"/>
@@ -5632,7 +5674,7 @@
         <v>4.4864500000000005</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>394</v>
       </c>
@@ -5647,11 +5689,11 @@
       </c>
       <c r="E53" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505401,94 </v>
+        <v xml:space="preserve">505401.94 </v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042915,05 </v>
+        <v xml:space="preserve">0042915.05 </v>
       </c>
       <c r="G53">
         <f t="shared" si="11"/>
@@ -5686,7 +5728,7 @@
         <v>4.4875138888888895</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>394</v>
       </c>
@@ -5701,11 +5743,11 @@
       </c>
       <c r="E54" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505402,90 </v>
+        <v xml:space="preserve">505402.90 </v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042918,38 </v>
+        <v xml:space="preserve">0042918.38 </v>
       </c>
       <c r="G54">
         <f t="shared" si="11"/>
@@ -5740,7 +5782,7 @@
         <v>4.4884388888888882</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>394</v>
       </c>
@@ -5755,11 +5797,11 @@
       </c>
       <c r="E55" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505403,86 </v>
+        <v xml:space="preserve">505403.86 </v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042921,69 </v>
+        <v xml:space="preserve">0042921.69 </v>
       </c>
       <c r="G55">
         <f t="shared" si="11"/>
@@ -5794,7 +5836,7 @@
         <v>4.4893583333333344</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>394</v>
       </c>
@@ -5809,11 +5851,11 @@
       </c>
       <c r="E56" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505403,96 </v>
+        <v xml:space="preserve">505403.96 </v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042920,72 </v>
+        <v xml:space="preserve">0042920.72 </v>
       </c>
       <c r="G56">
         <f t="shared" si="11"/>
@@ -5848,7 +5890,7 @@
         <v>4.4890888888888894</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>394</v>
       </c>
@@ -5863,11 +5905,11 @@
       </c>
       <c r="E57" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505404,40 </v>
+        <v xml:space="preserve">505404.40 </v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042922,68 </v>
+        <v xml:space="preserve">0042922.68 </v>
       </c>
       <c r="G57">
         <f t="shared" si="11"/>
@@ -5902,7 +5944,7 @@
         <v>4.4896333333333338</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>394</v>
       </c>
@@ -5917,11 +5959,11 @@
       </c>
       <c r="E58" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505404,96 </v>
+        <v xml:space="preserve">505404.96 </v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042925,49 </v>
+        <v xml:space="preserve">0042925.49 </v>
       </c>
       <c r="G58">
         <f t="shared" si="11"/>
@@ -5956,7 +5998,7 @@
         <v>4.490413888888888</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>394</v>
       </c>
@@ -5971,11 +6013,11 @@
       </c>
       <c r="E59" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505405,05 </v>
+        <v xml:space="preserve">505405.05 </v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042924,51 </v>
+        <v xml:space="preserve">0042924.51 </v>
       </c>
       <c r="G59">
         <f t="shared" si="11"/>
@@ -6010,7 +6052,7 @@
         <v>4.4901416666666671</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>394</v>
       </c>
@@ -6025,11 +6067,11 @@
       </c>
       <c r="E60" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505405,54 </v>
+        <v xml:space="preserve">505405.54 </v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042926,45 </v>
+        <v xml:space="preserve">0042926.45 </v>
       </c>
       <c r="G60">
         <f t="shared" si="11"/>
@@ -6064,7 +6106,7 @@
         <v>4.4906805555555547</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>394</v>
       </c>
@@ -6079,11 +6121,11 @@
       </c>
       <c r="E61" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505406,06 </v>
+        <v xml:space="preserve">505406.06 </v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042929,29 </v>
+        <v xml:space="preserve">0042929.29 </v>
       </c>
       <c r="G61">
         <f t="shared" si="11"/>
@@ -6118,7 +6160,7 @@
         <v>4.4914694444444452</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>394</v>
       </c>
@@ -6133,11 +6175,11 @@
       </c>
       <c r="E62" t="str">
         <f t="shared" si="3"/>
-        <v>505406,87</v>
+        <v>505406.87</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="4"/>
-        <v>0042931,29</v>
+        <v>0042931.29</v>
       </c>
       <c r="G62">
         <f t="shared" si="11"/>
@@ -6172,7 +6214,7 @@
         <v>4.4920249999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>395</v>
       </c>
@@ -6187,11 +6229,11 @@
       </c>
       <c r="E63" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505356,03 </v>
+        <v xml:space="preserve">505356.03 </v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042906,97 </v>
+        <v xml:space="preserve">0042906.97 </v>
       </c>
       <c r="G63">
         <f t="shared" si="11"/>
@@ -6226,7 +6268,7 @@
         <v>4.4852694444444445</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>395</v>
       </c>
@@ -6241,11 +6283,11 @@
       </c>
       <c r="E64" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505357,45 </v>
+        <v xml:space="preserve">505357.45 </v>
       </c>
       <c r="F64" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042909,40 </v>
+        <v xml:space="preserve">0042909.40 </v>
       </c>
       <c r="G64">
         <f t="shared" si="11"/>
@@ -6280,7 +6322,7 @@
         <v>4.4859444444444447</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>395</v>
       </c>
@@ -6295,11 +6337,11 @@
       </c>
       <c r="E65" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505357,57 </v>
+        <v xml:space="preserve">505357.57 </v>
       </c>
       <c r="F65" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042910,24 </v>
+        <v xml:space="preserve">0042910.24 </v>
       </c>
       <c r="G65">
         <f t="shared" si="11"/>
@@ -6334,7 +6376,7 @@
         <v>4.4861777777777769</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>395</v>
       </c>
@@ -6349,11 +6391,11 @@
       </c>
       <c r="E66" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">505358,20 </v>
+        <v xml:space="preserve">505358.20 </v>
       </c>
       <c r="F66" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">0042912,07 </v>
+        <v xml:space="preserve">0042912.07 </v>
       </c>
       <c r="G66">
         <f t="shared" ref="G66:G97" si="14">_xlfn.FLOOR.MATH(E66/10000)</f>
@@ -6388,7 +6430,7 @@
         <v>4.4866861111111112</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>395</v>
       </c>
@@ -6402,12 +6444,12 @@
         <v>356</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E130" si="17">SUBSTITUTE( SUBSTITUTE(C67,"N",""),".",",")</f>
-        <v xml:space="preserve">505358,71 </v>
+        <f t="shared" ref="E67:E130" si="17">SUBSTITUTE( SUBSTITUTE(C67,"N",""),",",".")</f>
+        <v xml:space="preserve">505358.71 </v>
       </c>
       <c r="F67" t="str">
-        <f t="shared" ref="F67:F130" si="18">SUBSTITUTE( SUBSTITUTE(D67,"E",""),".",",")</f>
-        <v xml:space="preserve">0042914,00 </v>
+        <f t="shared" ref="F67:F130" si="18">SUBSTITUTE( SUBSTITUTE(D67,"E",""),",",".")</f>
+        <v xml:space="preserve">0042914.00 </v>
       </c>
       <c r="G67">
         <f t="shared" si="14"/>
@@ -6442,7 +6484,7 @@
         <v>4.487222222222222</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>395</v>
       </c>
@@ -6457,11 +6499,11 @@
       </c>
       <c r="E68" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">505359,10 </v>
+        <v xml:space="preserve">505359.10 </v>
       </c>
       <c r="F68" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">0042915,10 </v>
+        <v xml:space="preserve">0042915.10 </v>
       </c>
       <c r="G68">
         <f t="shared" si="14"/>
@@ -6496,7 +6538,7 @@
         <v>4.4875277777777773</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>395</v>
       </c>
@@ -6511,11 +6553,11 @@
       </c>
       <c r="E69" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">505359,17 </v>
+        <v xml:space="preserve">505359.17 </v>
       </c>
       <c r="F69" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">0042915,97 </v>
+        <v xml:space="preserve">0042915.97 </v>
       </c>
       <c r="G69">
         <f t="shared" si="14"/>
@@ -6550,7 +6592,7 @@
         <v>4.4877694444444449</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>395</v>
       </c>
@@ -6565,11 +6607,11 @@
       </c>
       <c r="E70" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">505359,76 </v>
+        <v xml:space="preserve">505359.76 </v>
       </c>
       <c r="F70" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">0042917,83 </v>
+        <v xml:space="preserve">0042917.83 </v>
       </c>
       <c r="G70">
         <f t="shared" si="14"/>
@@ -6604,7 +6646,7 @@
         <v>4.4882861111111119</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>395</v>
       </c>
@@ -6619,11 +6661,11 @@
       </c>
       <c r="E71" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">505400,19 </v>
+        <v xml:space="preserve">505400.19 </v>
       </c>
       <c r="F71" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">0042918,89 </v>
+        <v xml:space="preserve">0042918.89 </v>
       </c>
       <c r="G71">
         <f t="shared" si="14"/>
@@ -6658,7 +6700,7 @@
         <v>4.4885805555555551</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>395</v>
       </c>
@@ -6673,11 +6715,11 @@
       </c>
       <c r="E72" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">505400,26 </v>
+        <v xml:space="preserve">505400.26 </v>
       </c>
       <c r="F72" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">0042919,75 </v>
+        <v xml:space="preserve">0042919.75 </v>
       </c>
       <c r="G72">
         <f t="shared" si="14"/>
@@ -6712,7 +6754,7 @@
         <v>4.4888194444444443</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>395</v>
       </c>
@@ -6727,11 +6769,11 @@
       </c>
       <c r="E73" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">505400,86 </v>
+        <v xml:space="preserve">505400.86 </v>
       </c>
       <c r="F73" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">0042921,62 </v>
+        <v xml:space="preserve">0042921.62 </v>
       </c>
       <c r="G73">
         <f t="shared" si="14"/>
@@ -6766,7 +6808,7 @@
         <v>4.4893388888888897</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>395</v>
       </c>
@@ -6781,11 +6823,11 @@
       </c>
       <c r="E74" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">505401,29 </v>
+        <v xml:space="preserve">505401.29 </v>
       </c>
       <c r="F74" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">0042922,69 </v>
+        <v xml:space="preserve">0042922.69 </v>
       </c>
       <c r="G74">
         <f t="shared" si="14"/>
@@ -6820,7 +6862,7 @@
         <v>4.4896361111111114</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>395</v>
       </c>
@@ -6835,11 +6877,11 @@
       </c>
       <c r="E75" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">505401,36 </v>
+        <v xml:space="preserve">505401.36 </v>
       </c>
       <c r="F75" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">0042923,56 </v>
+        <v xml:space="preserve">0042923.56 </v>
       </c>
       <c r="G75">
         <f t="shared" si="14"/>
@@ -6874,7 +6916,7 @@
         <v>4.4898777777777772</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>395</v>
       </c>
@@ -6889,11 +6931,11 @@
       </c>
       <c r="E76" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">505401,13 </v>
+        <v xml:space="preserve">505401.13 </v>
       </c>
       <c r="F76" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">0042926,01 </v>
+        <v xml:space="preserve">0042926.01 </v>
       </c>
       <c r="G76">
         <f t="shared" si="14"/>
@@ -6928,7 +6970,7 @@
         <v>4.4905583333333343</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>395</v>
       </c>
@@ -6943,11 +6985,11 @@
       </c>
       <c r="E77" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">505402,31 </v>
+        <v xml:space="preserve">505402.31 </v>
       </c>
       <c r="F77" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">0042926,63 </v>
+        <v xml:space="preserve">0042926.63 </v>
       </c>
       <c r="G77">
         <f t="shared" si="14"/>
@@ -6982,7 +7024,7 @@
         <v>4.4907305555555546</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>395</v>
       </c>
@@ -6997,11 +7039,11 @@
       </c>
       <c r="E78" t="str">
         <f t="shared" si="17"/>
-        <v xml:space="preserve">505402,47 </v>
+        <v xml:space="preserve">505402.47 </v>
       </c>
       <c r="F78" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">0042927,34 </v>
+        <v xml:space="preserve">0042927.34 </v>
       </c>
       <c r="G78">
         <f t="shared" si="14"/>
@@ -7036,7 +7078,7 @@
         <v>4.4909277777777765</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>395</v>
       </c>
@@ -7051,11 +7093,11 @@
       </c>
       <c r="E79" t="str">
         <f t="shared" si="17"/>
-        <v>505403,56</v>
+        <v>505403.56</v>
       </c>
       <c r="F79" t="str">
         <f t="shared" si="18"/>
-        <v>0042930,23</v>
+        <v>0042930.23</v>
       </c>
       <c r="G79">
         <f t="shared" si="14"/>
@@ -7090,7 +7132,7 @@
         <v>4.4917305555555567</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>396</v>
       </c>
@@ -7105,11 +7147,11 @@
       </c>
       <c r="E80" t="str">
         <f t="shared" si="17"/>
-        <v>505347,41</v>
+        <v>505347.41</v>
       </c>
       <c r="F80" t="str">
         <f t="shared" si="18"/>
-        <v>0042915,32</v>
+        <v>0042915.32</v>
       </c>
       <c r="G80">
         <f t="shared" si="14"/>
@@ -7144,7 +7186,7 @@
         <v>4.4875888888888893</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>396</v>
       </c>
@@ -7159,11 +7201,11 @@
       </c>
       <c r="E81" t="str">
         <f t="shared" si="17"/>
-        <v>505345,42</v>
+        <v>505345.42</v>
       </c>
       <c r="F81" t="str">
         <f t="shared" si="18"/>
-        <v>0042917,17</v>
+        <v>0042917.17</v>
       </c>
       <c r="G81">
         <f t="shared" si="14"/>
@@ -7198,7 +7240,7 @@
         <v>4.4881027777777778</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>396</v>
       </c>
@@ -7213,11 +7255,11 @@
       </c>
       <c r="E82" t="str">
         <f t="shared" si="17"/>
-        <v>505348,79</v>
+        <v>505348.79</v>
       </c>
       <c r="F82" t="str">
         <f t="shared" si="18"/>
-        <v>0042918,92</v>
+        <v>0042918.92</v>
       </c>
       <c r="G82">
         <f t="shared" si="14"/>
@@ -7252,7 +7294,7 @@
         <v>4.4885888888888887</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>396</v>
       </c>
@@ -7267,11 +7309,11 @@
       </c>
       <c r="E83" t="str">
         <f t="shared" si="17"/>
-        <v>505345,97</v>
+        <v>505345.97</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="18"/>
-        <v>0042919,08</v>
+        <v>0042919.08</v>
       </c>
       <c r="G83">
         <f t="shared" si="14"/>
@@ -7306,7 +7348,7 @@
         <v>4.4886333333333335</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>396</v>
       </c>
@@ -7321,11 +7363,11 @@
       </c>
       <c r="E84" t="str">
         <f t="shared" si="17"/>
-        <v>505348,39</v>
+        <v>505348.39</v>
       </c>
       <c r="F84" t="str">
         <f t="shared" si="18"/>
-        <v>0042918,70</v>
+        <v>0042918.70</v>
       </c>
       <c r="G84">
         <f t="shared" si="14"/>
@@ -7360,7 +7402,7 @@
         <v>4.4885277777777768</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>396</v>
       </c>
@@ -7375,11 +7417,11 @@
       </c>
       <c r="E85" t="str">
         <f t="shared" si="17"/>
-        <v>505346,84</v>
+        <v>505346.84</v>
       </c>
       <c r="F85" t="str">
         <f t="shared" si="18"/>
-        <v>0042918,91</v>
+        <v>0042918.91</v>
       </c>
       <c r="G85">
         <f t="shared" si="14"/>
@@ -7414,7 +7456,7 @@
         <v>4.4885861111111121</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>396</v>
       </c>
@@ -7429,11 +7471,11 @@
       </c>
       <c r="E86" t="str">
         <f t="shared" si="17"/>
-        <v>505349,38</v>
+        <v>505349.38</v>
       </c>
       <c r="F86" t="str">
         <f t="shared" si="18"/>
-        <v>0042918,97</v>
+        <v>0042918.97</v>
       </c>
       <c r="G86">
         <f t="shared" si="14"/>
@@ -7468,7 +7510,7 @@
         <v>4.4886027777777784</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>396</v>
       </c>
@@ -7483,11 +7525,11 @@
       </c>
       <c r="E87" t="str">
         <f t="shared" si="17"/>
-        <v>505346,51</v>
+        <v>505346.51</v>
       </c>
       <c r="F87" t="str">
         <f t="shared" si="18"/>
-        <v>0042920,54</v>
+        <v>0042920.54</v>
       </c>
       <c r="G87">
         <f t="shared" si="14"/>
@@ -7522,7 +7564,7 @@
         <v>4.4890388888888895</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>396</v>
       </c>
@@ -7537,11 +7579,11 @@
       </c>
       <c r="E88" t="str">
         <f t="shared" si="17"/>
-        <v>505349,92</v>
+        <v>505349.92</v>
       </c>
       <c r="F88" t="str">
         <f t="shared" si="18"/>
-        <v>0042920,85</v>
+        <v>0042920.85</v>
       </c>
       <c r="G88">
         <f t="shared" si="14"/>
@@ -7576,7 +7618,7 @@
         <v>4.4891249999999996</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>396</v>
       </c>
@@ -7591,11 +7633,11 @@
       </c>
       <c r="E89" t="str">
         <f t="shared" si="17"/>
-        <v>505347,81</v>
+        <v>505347.81</v>
       </c>
       <c r="F89" t="str">
         <f t="shared" si="18"/>
-        <v>0042922,28</v>
+        <v>0042922.28</v>
       </c>
       <c r="G89">
         <f t="shared" si="14"/>
@@ -7630,7 +7672,7 @@
         <v>4.489522222222222</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>396</v>
       </c>
@@ -7645,11 +7687,11 @@
       </c>
       <c r="E90" t="str">
         <f t="shared" si="17"/>
-        <v>505349,48</v>
+        <v>505349.48</v>
       </c>
       <c r="F90" t="str">
         <f t="shared" si="18"/>
-        <v>0042922,61</v>
+        <v>0042922.61</v>
       </c>
       <c r="G90">
         <f t="shared" si="14"/>
@@ -7684,7 +7726,7 @@
         <v>4.489613888888889</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>396</v>
       </c>
@@ -7699,11 +7741,11 @@
       </c>
       <c r="E91" t="str">
         <f t="shared" si="17"/>
-        <v>505348,61</v>
+        <v>505348.61</v>
       </c>
       <c r="F91" t="str">
         <f t="shared" si="18"/>
-        <v>0042924,97</v>
+        <v>0042924.97</v>
       </c>
       <c r="G91">
         <f t="shared" si="14"/>
@@ -7738,7 +7780,7 @@
         <v>4.4902694444444444</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>396</v>
       </c>
@@ -7753,11 +7795,11 @@
       </c>
       <c r="E92" t="str">
         <f t="shared" si="17"/>
-        <v>505350,47</v>
+        <v>505350.47</v>
       </c>
       <c r="F92" t="str">
         <f t="shared" si="18"/>
-        <v>0042922,74</v>
+        <v>0042922.74</v>
       </c>
       <c r="G92">
         <f t="shared" si="14"/>
@@ -7792,7 +7834,7 @@
         <v>4.4896499999999993</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>396</v>
       </c>
@@ -7807,11 +7849,11 @@
       </c>
       <c r="E93" t="str">
         <f t="shared" si="17"/>
-        <v>505351,15</v>
+        <v>505351.15</v>
       </c>
       <c r="F93" t="str">
         <f t="shared" si="18"/>
-        <v>0042925,11</v>
+        <v>0042925.11</v>
       </c>
       <c r="G93">
         <f t="shared" si="14"/>
@@ -7846,7 +7888,7 @@
         <v>4.4903083333333331</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>396</v>
       </c>
@@ -7861,11 +7903,11 @@
       </c>
       <c r="E94" t="str">
         <f t="shared" si="17"/>
-        <v>505350,78</v>
+        <v>505350.78</v>
       </c>
       <c r="F94" t="str">
         <f t="shared" si="18"/>
-        <v>0042927,03</v>
+        <v>0042927.03</v>
       </c>
       <c r="G94">
         <f t="shared" si="14"/>
@@ -7900,7 +7942,7 @@
         <v>4.4908416666666664</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>396</v>
       </c>
@@ -7915,11 +7957,11 @@
       </c>
       <c r="E95" t="str">
         <f t="shared" si="17"/>
-        <v>505351,90</v>
+        <v>505351.90</v>
       </c>
       <c r="F95" t="str">
         <f t="shared" si="18"/>
-        <v>0042927,72</v>
+        <v>0042927.72</v>
       </c>
       <c r="G95">
         <f t="shared" si="14"/>
@@ -7954,7 +7996,7 @@
         <v>4.4910333333333341</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>397</v>
       </c>
@@ -7969,11 +8011,11 @@
       </c>
       <c r="E96" t="str">
         <f t="shared" si="17"/>
-        <v>505339,45</v>
+        <v>505339.45</v>
       </c>
       <c r="F96" t="str">
         <f t="shared" si="18"/>
-        <v>0042918,18</v>
+        <v>0042918.18</v>
       </c>
       <c r="G96">
         <f t="shared" si="14"/>
@@ -8008,7 +8050,7 @@
         <v>4.4883833333333332</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>397</v>
       </c>
@@ -8023,11 +8065,11 @@
       </c>
       <c r="E97" t="str">
         <f t="shared" si="17"/>
-        <v>505338,44</v>
+        <v>505338.44</v>
       </c>
       <c r="F97" t="str">
         <f t="shared" si="18"/>
-        <v>0042916,88</v>
+        <v>0042916.88</v>
       </c>
       <c r="G97">
         <f t="shared" si="14"/>
@@ -8062,7 +8104,7 @@
         <v>4.4880222222222219</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>397</v>
       </c>
@@ -8077,11 +8119,11 @@
       </c>
       <c r="E98" t="str">
         <f t="shared" si="17"/>
-        <v>505338,91</v>
+        <v>505338.91</v>
       </c>
       <c r="F98" t="str">
         <f t="shared" si="18"/>
-        <v>0047914,71</v>
+        <v>0047914.71</v>
       </c>
       <c r="G98">
         <f t="shared" ref="G98:G129" si="24">_xlfn.FLOOR.MATH(E98/10000)</f>
@@ -8116,7 +8158,7 @@
         <v>5.320752777777777</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>397</v>
       </c>
@@ -8131,11 +8173,11 @@
       </c>
       <c r="E99" t="str">
         <f t="shared" si="17"/>
-        <v>505341,15</v>
+        <v>505341.15</v>
       </c>
       <c r="F99" t="str">
         <f t="shared" si="18"/>
-        <v>0042919,76</v>
+        <v>0042919.76</v>
       </c>
       <c r="G99">
         <f t="shared" si="24"/>
@@ -8170,7 +8212,7 @@
         <v>4.4888222222222227</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>398</v>
       </c>
@@ -8185,11 +8227,11 @@
       </c>
       <c r="E100" t="str">
         <f t="shared" si="17"/>
-        <v>505335,23</v>
+        <v>505335.23</v>
       </c>
       <c r="F100" t="str">
         <f t="shared" si="18"/>
-        <v>0042910,85</v>
+        <v>0042910.85</v>
       </c>
       <c r="G100">
         <f t="shared" si="24"/>
@@ -8224,7 +8266,7 @@
         <v>4.4863472222222223</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>398</v>
       </c>
@@ -8239,11 +8281,11 @@
       </c>
       <c r="E101" t="str">
         <f t="shared" si="17"/>
-        <v>505336,34</v>
+        <v>505336.34</v>
       </c>
       <c r="F101" t="str">
         <f t="shared" si="18"/>
-        <v>0042910,21</v>
+        <v>0042910.21</v>
       </c>
       <c r="G101">
         <f t="shared" si="24"/>
@@ -8278,7 +8320,7 @@
         <v>4.4861694444444442</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>398</v>
       </c>
@@ -8293,11 +8335,11 @@
       </c>
       <c r="E102" t="str">
         <f t="shared" si="17"/>
-        <v>505337,78</v>
+        <v>505337.78</v>
       </c>
       <c r="F102" t="str">
         <f t="shared" si="18"/>
-        <v>0042909,37</v>
+        <v>0042909.37</v>
       </c>
       <c r="G102">
         <f t="shared" si="24"/>
@@ -8332,7 +8374,7 @@
         <v>4.485936111111112</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>398</v>
       </c>
@@ -8347,11 +8389,11 @@
       </c>
       <c r="E103" t="str">
         <f t="shared" si="17"/>
-        <v>505334,54</v>
+        <v>505334.54</v>
       </c>
       <c r="F103" t="str">
         <f t="shared" si="18"/>
-        <v>0042906,26</v>
+        <v>0042906.26</v>
       </c>
       <c r="G103">
         <f t="shared" si="24"/>
@@ -8386,7 +8428,7 @@
         <v>4.4850722222222226</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>398</v>
       </c>
@@ -8401,11 +8443,11 @@
       </c>
       <c r="E104" t="str">
         <f t="shared" si="17"/>
-        <v>505335,66</v>
+        <v>505335.66</v>
       </c>
       <c r="F104" t="str">
         <f t="shared" si="18"/>
-        <v>0042905,62</v>
+        <v>0042905.62</v>
       </c>
       <c r="G104">
         <f t="shared" si="24"/>
@@ -8440,7 +8482,7 @@
         <v>4.4848944444444454</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>398</v>
       </c>
@@ -8455,11 +8497,11 @@
       </c>
       <c r="E105" t="str">
         <f t="shared" si="17"/>
-        <v>505337,14</v>
+        <v>505337.14</v>
       </c>
       <c r="F105" t="str">
         <f t="shared" si="18"/>
-        <v>0042904,77</v>
+        <v>0042904.77</v>
       </c>
       <c r="G105">
         <f t="shared" si="24"/>
@@ -8494,7 +8536,7 @@
         <v>4.4846583333333321</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>398</v>
       </c>
@@ -8509,7 +8551,7 @@
       </c>
       <c r="E106" t="str">
         <f t="shared" si="17"/>
-        <v>505333,11</v>
+        <v>505333.11</v>
       </c>
       <c r="F106" t="str">
         <f t="shared" si="18"/>
@@ -8548,7 +8590,7 @@
         <v>6129.0402777777772</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>398</v>
       </c>
@@ -8563,11 +8605,11 @@
       </c>
       <c r="E107" t="str">
         <f t="shared" si="17"/>
-        <v>505334,43</v>
+        <v>505334.43</v>
       </c>
       <c r="F107" t="str">
         <f t="shared" si="18"/>
-        <v>0042900,89</v>
+        <v>0042900.89</v>
       </c>
       <c r="G107">
         <f t="shared" si="24"/>
@@ -8602,7 +8644,7 @@
         <v>4.4835805555555552</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>398</v>
       </c>
@@ -8617,11 +8659,11 @@
       </c>
       <c r="E108" t="str">
         <f t="shared" si="17"/>
-        <v>505335,95</v>
+        <v>505335.95</v>
       </c>
       <c r="F108" t="str">
         <f t="shared" si="18"/>
-        <v>0042900,01</v>
+        <v>0042900.01</v>
       </c>
       <c r="G108">
         <f t="shared" si="24"/>
@@ -8656,7 +8698,7 @@
         <v>4.4833361111111119</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>400</v>
       </c>
@@ -8671,11 +8713,11 @@
       </c>
       <c r="E109" t="str">
         <f t="shared" si="17"/>
-        <v>505358,74</v>
+        <v>505358.74</v>
       </c>
       <c r="F109" t="str">
         <f t="shared" si="18"/>
-        <v>0042837,76</v>
+        <v>0042837.76</v>
       </c>
       <c r="G109">
         <f t="shared" si="24"/>
@@ -8710,7 +8752,7 @@
         <v>4.477155555555556</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>400</v>
       </c>
@@ -8725,11 +8767,11 @@
       </c>
       <c r="E110" t="str">
         <f t="shared" si="17"/>
-        <v>505356,41</v>
+        <v>505356.41</v>
       </c>
       <c r="F110" t="str">
         <f t="shared" si="18"/>
-        <v>0042836,80</v>
+        <v>0042836.80</v>
       </c>
       <c r="G110">
         <f t="shared" si="24"/>
@@ -8764,7 +8806,7 @@
         <v>4.4768888888888902</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>400</v>
       </c>
@@ -8779,11 +8821,11 @@
       </c>
       <c r="E111" t="str">
         <f t="shared" si="17"/>
-        <v>505355,55</v>
+        <v>505355.55</v>
       </c>
       <c r="F111" t="str">
         <f t="shared" si="18"/>
-        <v>0042836,44</v>
+        <v>0042836.44</v>
       </c>
       <c r="G111">
         <f t="shared" si="24"/>
@@ -8818,7 +8860,7 @@
         <v>4.4767888888888896</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>400</v>
       </c>
@@ -8833,11 +8875,11 @@
       </c>
       <c r="E112" t="str">
         <f t="shared" si="17"/>
-        <v>505355,81</v>
+        <v>505355.81</v>
       </c>
       <c r="F112" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">0042834,71 </v>
+        <v xml:space="preserve">0042834.71 </v>
       </c>
       <c r="G112">
         <f t="shared" si="24"/>
@@ -8872,7 +8914,7 @@
         <v>4.4763083333333329</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>400</v>
       </c>
@@ -8887,11 +8929,11 @@
       </c>
       <c r="E113" t="str">
         <f t="shared" si="17"/>
-        <v>505354,58</v>
+        <v>505354.58</v>
       </c>
       <c r="F113" t="str">
         <f t="shared" si="18"/>
-        <v>0042833,06</v>
+        <v>0042833.06</v>
       </c>
       <c r="G113">
         <f t="shared" si="24"/>
@@ -8926,7 +8968,7 @@
         <v>4.4758499999999994</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>400</v>
       </c>
@@ -8941,11 +8983,11 @@
       </c>
       <c r="E114" t="str">
         <f t="shared" si="17"/>
-        <v>505354,60</v>
+        <v>505354.60</v>
       </c>
       <c r="F114" t="str">
         <f t="shared" si="18"/>
-        <v>0042830,52</v>
+        <v>0042830.52</v>
       </c>
       <c r="G114">
         <f t="shared" si="24"/>
@@ -8980,7 +9022,7 @@
         <v>4.4751444444444433</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>400</v>
       </c>
@@ -8995,11 +9037,11 @@
       </c>
       <c r="E115" t="str">
         <f t="shared" si="17"/>
-        <v>505353,60</v>
+        <v>505353.60</v>
       </c>
       <c r="F115" t="str">
         <f t="shared" si="18"/>
-        <v>0042829,69</v>
+        <v>0042829.69</v>
       </c>
       <c r="G115">
         <f t="shared" si="24"/>
@@ -9034,7 +9076,7 @@
         <v>4.4749138888888895</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>400</v>
       </c>
@@ -9049,11 +9091,11 @@
       </c>
       <c r="E116" t="str">
         <f t="shared" si="17"/>
-        <v>505353,99</v>
+        <v>505353.99</v>
       </c>
       <c r="F116" t="str">
         <f t="shared" si="18"/>
-        <v>0042828,42</v>
+        <v>0042828.42</v>
       </c>
       <c r="G116">
         <f t="shared" si="24"/>
@@ -9088,7 +9130,7 @@
         <v>4.474561111111111</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>400</v>
       </c>
@@ -9103,11 +9145,11 @@
       </c>
       <c r="E117" t="str">
         <f t="shared" si="17"/>
-        <v>505352,69</v>
+        <v>505352.69</v>
       </c>
       <c r="F117" t="str">
         <f t="shared" si="18"/>
-        <v>0042826,29</v>
+        <v>0042826.29</v>
       </c>
       <c r="G117">
         <f t="shared" si="24"/>
@@ -9142,7 +9184,7 @@
         <v>4.4739694444444451</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>401</v>
       </c>
@@ -9157,11 +9199,11 @@
       </c>
       <c r="E118" t="str">
         <f t="shared" si="17"/>
-        <v>505350,77</v>
+        <v>505350.77</v>
       </c>
       <c r="F118" t="str">
         <f t="shared" si="18"/>
-        <v>0042821,85</v>
+        <v>0042821.85</v>
       </c>
       <c r="G118">
         <f t="shared" si="24"/>
@@ -9196,7 +9238,7 @@
         <v>4.4727361111111108</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>401</v>
       </c>
@@ -9211,11 +9253,11 @@
       </c>
       <c r="E119" t="str">
         <f t="shared" si="17"/>
-        <v>505350,55</v>
+        <v>505350.55</v>
       </c>
       <c r="F119" t="str">
         <f t="shared" si="18"/>
-        <v>0042821,70</v>
+        <v>0042821.70</v>
       </c>
       <c r="G119">
         <f t="shared" si="24"/>
@@ -9250,7 +9292,7 @@
         <v>4.4726944444444436</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>401</v>
       </c>
@@ -9265,11 +9307,11 @@
       </c>
       <c r="E120" t="str">
         <f t="shared" si="17"/>
-        <v>505350,51</v>
+        <v>505350.51</v>
       </c>
       <c r="F120" t="str">
         <f t="shared" si="18"/>
-        <v>0042821,02</v>
+        <v>0042821.02</v>
       </c>
       <c r="G120">
         <f t="shared" si="24"/>
@@ -9304,7 +9346,7 @@
         <v>4.4725055555555544</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>401</v>
       </c>
@@ -9319,11 +9361,11 @@
       </c>
       <c r="E121" t="str">
         <f t="shared" si="17"/>
-        <v>505350,16</v>
+        <v>505350.16</v>
       </c>
       <c r="F121" t="str">
         <f t="shared" si="18"/>
-        <v>0042820,47</v>
+        <v>0042820.47</v>
       </c>
       <c r="G121">
         <f t="shared" si="24"/>
@@ -9358,7 +9400,7 @@
         <v>4.4723527777777781</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>401</v>
       </c>
@@ -9373,11 +9415,11 @@
       </c>
       <c r="E122" t="str">
         <f t="shared" si="17"/>
-        <v>505350,25</v>
+        <v>505350.25</v>
       </c>
       <c r="F122" t="str">
         <f t="shared" si="18"/>
-        <v>0042820,20</v>
+        <v>0042820.20</v>
       </c>
       <c r="G122">
         <f t="shared" si="24"/>
@@ -9412,7 +9454,7 @@
         <v>4.4722777777777774</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>401</v>
       </c>
@@ -9427,11 +9469,11 @@
       </c>
       <c r="E123" t="str">
         <f t="shared" si="17"/>
-        <v>505349,93</v>
+        <v>505349.93</v>
       </c>
       <c r="F123" t="str">
         <f t="shared" si="18"/>
-        <v>0042819,19</v>
+        <v>0042819.19</v>
       </c>
       <c r="G123">
         <f t="shared" si="24"/>
@@ -9466,7 +9508,7 @@
         <v>4.4719972222222228</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>401</v>
       </c>
@@ -9481,11 +9523,11 @@
       </c>
       <c r="E124" t="str">
         <f t="shared" si="17"/>
-        <v>505349,71</v>
+        <v>505349.71</v>
       </c>
       <c r="F124" t="str">
         <f t="shared" si="18"/>
-        <v>0042819,05</v>
+        <v>0042819.05</v>
       </c>
       <c r="G124">
         <f t="shared" si="24"/>
@@ -9520,7 +9562,7 @@
         <v>4.4719583333333341</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>401</v>
       </c>
@@ -9535,11 +9577,11 @@
       </c>
       <c r="E125" t="str">
         <f t="shared" si="17"/>
-        <v>505349,67</v>
+        <v>505349.67</v>
       </c>
       <c r="F125" t="str">
         <f t="shared" si="18"/>
-        <v>0042818,37</v>
+        <v>0042818.37</v>
       </c>
       <c r="G125">
         <f t="shared" si="24"/>
@@ -9574,7 +9616,7 @@
         <v>4.4717694444444449</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>401</v>
       </c>
@@ -9589,11 +9631,11 @@
       </c>
       <c r="E126" t="str">
         <f t="shared" si="17"/>
-        <v>505349,32</v>
+        <v>505349.32</v>
       </c>
       <c r="F126" t="str">
         <f t="shared" si="18"/>
-        <v xml:space="preserve">0042817,81 </v>
+        <v xml:space="preserve">0042817.81 </v>
       </c>
       <c r="G126">
         <f t="shared" si="24"/>
@@ -9628,7 +9670,7 @@
         <v>4.4716138888888883</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>401</v>
       </c>
@@ -9643,11 +9685,11 @@
       </c>
       <c r="E127" t="str">
         <f t="shared" si="17"/>
-        <v>505349,40</v>
+        <v>505349.40</v>
       </c>
       <c r="F127" t="str">
         <f t="shared" si="18"/>
-        <v>0042817,54</v>
+        <v>0042817.54</v>
       </c>
       <c r="G127">
         <f t="shared" si="24"/>
@@ -9682,7 +9724,7 @@
         <v>4.4715388888888894</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>401</v>
       </c>
@@ -9697,11 +9739,11 @@
       </c>
       <c r="E128" t="str">
         <f t="shared" si="17"/>
-        <v>505349,14</v>
+        <v>505349.14</v>
       </c>
       <c r="F128" t="str">
         <f t="shared" si="18"/>
-        <v>0042816,73</v>
+        <v>0042816.73</v>
       </c>
       <c r="G128">
         <f t="shared" si="24"/>
@@ -9736,7 +9778,7 @@
         <v>4.4713138888888899</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>401</v>
       </c>
@@ -9751,11 +9793,11 @@
       </c>
       <c r="E129" t="str">
         <f t="shared" si="17"/>
-        <v>505348,93</v>
+        <v>505348.93</v>
       </c>
       <c r="F129" t="str">
         <f t="shared" si="18"/>
-        <v>0042816,58</v>
+        <v>0042816.58</v>
       </c>
       <c r="G129">
         <f t="shared" si="24"/>
@@ -9790,7 +9832,7 @@
         <v>4.4712722222222228</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>401</v>
       </c>
@@ -9805,11 +9847,11 @@
       </c>
       <c r="E130" t="str">
         <f t="shared" si="17"/>
-        <v>505348,88</v>
+        <v>505348.88</v>
       </c>
       <c r="F130" t="str">
         <f t="shared" si="18"/>
-        <v>0042815,90</v>
+        <v>0042815.90</v>
       </c>
       <c r="G130">
         <f t="shared" ref="G130:G161" si="27">_xlfn.FLOOR.MATH(E130/10000)</f>
@@ -9844,7 +9886,7 @@
         <v>4.4710833333333335</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>401</v>
       </c>
@@ -9858,12 +9900,12 @@
         <v>102</v>
       </c>
       <c r="E131" t="str">
-        <f t="shared" ref="E131:E177" si="30">SUBSTITUTE( SUBSTITUTE(C131,"N",""),".",",")</f>
-        <v>505348,53</v>
+        <f t="shared" ref="E131:E177" si="30">SUBSTITUTE( SUBSTITUTE(C131,"N",""),",",".")</f>
+        <v>505348.53</v>
       </c>
       <c r="F131" t="str">
-        <f t="shared" ref="F131:F177" si="31">SUBSTITUTE( SUBSTITUTE(D131,"E",""),".",",")</f>
-        <v>0042815,34</v>
+        <f t="shared" ref="F131:F177" si="31">SUBSTITUTE( SUBSTITUTE(D131,"E",""),",",".")</f>
+        <v>0042815.34</v>
       </c>
       <c r="G131">
         <f t="shared" si="27"/>
@@ -9898,7 +9940,7 @@
         <v>4.4709277777777769</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>401</v>
       </c>
@@ -9913,11 +9955,11 @@
       </c>
       <c r="E132" t="str">
         <f t="shared" si="30"/>
-        <v>505348,62</v>
+        <v>505348.62</v>
       </c>
       <c r="F132" t="str">
         <f t="shared" si="31"/>
-        <v>0042815,08</v>
+        <v>0042815.08</v>
       </c>
       <c r="G132">
         <f t="shared" si="27"/>
@@ -9952,7 +9994,7 @@
         <v>4.4708555555555565</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>401</v>
       </c>
@@ -9967,11 +10009,11 @@
       </c>
       <c r="E133" t="str">
         <f t="shared" si="30"/>
-        <v>505348,36</v>
+        <v>505348.36</v>
       </c>
       <c r="F133" t="str">
         <f t="shared" si="31"/>
-        <v>0042814,25</v>
+        <v>0042814.25</v>
       </c>
       <c r="G133">
         <f t="shared" si="27"/>
@@ -10006,7 +10048,7 @@
         <v>4.4706250000000001</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>401</v>
       </c>
@@ -10021,11 +10063,11 @@
       </c>
       <c r="E134" t="str">
         <f t="shared" si="30"/>
-        <v>505348,14</v>
+        <v>505348.14</v>
       </c>
       <c r="F134" t="str">
         <f t="shared" si="31"/>
-        <v>0042814,11</v>
+        <v>0042814.11</v>
       </c>
       <c r="G134">
         <f t="shared" si="27"/>
@@ -10060,7 +10102,7 @@
         <v>4.4705861111111114</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>401</v>
       </c>
@@ -10075,11 +10117,11 @@
       </c>
       <c r="E135" t="str">
         <f t="shared" si="30"/>
-        <v>505348,10</v>
+        <v>505348.10</v>
       </c>
       <c r="F135" t="str">
         <f t="shared" si="31"/>
-        <v>0042813,43</v>
+        <v>0042813.43</v>
       </c>
       <c r="G135">
         <f t="shared" si="27"/>
@@ -10114,7 +10156,7 @@
         <v>4.4703972222222221</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>401</v>
       </c>
@@ -10129,11 +10171,11 @@
       </c>
       <c r="E136" t="str">
         <f t="shared" si="30"/>
-        <v>505347,75</v>
+        <v>505347.75</v>
       </c>
       <c r="F136" t="str">
         <f t="shared" si="31"/>
-        <v>0042812,87</v>
+        <v>0042812.87</v>
       </c>
       <c r="G136">
         <f t="shared" si="27"/>
@@ -10168,7 +10210,7 @@
         <v>4.4702416666666673</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>401</v>
       </c>
@@ -10183,11 +10225,11 @@
       </c>
       <c r="E137" t="str">
         <f t="shared" si="30"/>
-        <v>505347,84</v>
+        <v>505347.84</v>
       </c>
       <c r="F137" t="str">
         <f t="shared" si="31"/>
-        <v>0042812,61</v>
+        <v>0042812.61</v>
       </c>
       <c r="G137">
         <f t="shared" si="27"/>
@@ -10222,7 +10264,7 @@
         <v>4.4701694444444451</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>402</v>
       </c>
@@ -10237,11 +10279,11 @@
       </c>
       <c r="E138" t="str">
         <f t="shared" si="30"/>
-        <v>505354,68</v>
+        <v>505354.68</v>
       </c>
       <c r="F138" t="str">
         <f t="shared" si="31"/>
-        <v>0042801,41</v>
+        <v>0042801.41</v>
       </c>
       <c r="G138">
         <f t="shared" si="27"/>
@@ -10276,7 +10318,7 @@
         <v>4.467058333333334</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>402</v>
       </c>
@@ -10291,11 +10333,11 @@
       </c>
       <c r="E139" t="str">
         <f t="shared" si="30"/>
-        <v>505353,32</v>
+        <v>505353.32</v>
       </c>
       <c r="F139" t="str">
         <f t="shared" si="31"/>
-        <v>0042802,39</v>
+        <v>0042802.39</v>
       </c>
       <c r="G139">
         <f t="shared" si="27"/>
@@ -10330,7 +10372,7 @@
         <v>4.4673305555555558</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>402</v>
       </c>
@@ -10345,11 +10387,11 @@
       </c>
       <c r="E140" t="str">
         <f t="shared" si="30"/>
-        <v>505355,25</v>
+        <v>505355.25</v>
       </c>
       <c r="F140" t="str">
         <f t="shared" si="31"/>
-        <v>0042803,39</v>
+        <v>0042803.39</v>
       </c>
       <c r="G140">
         <f t="shared" si="27"/>
@@ -10384,7 +10426,7 @@
         <v>4.4676083333333336</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>402</v>
       </c>
@@ -10399,11 +10441,11 @@
       </c>
       <c r="E141" t="str">
         <f t="shared" si="30"/>
-        <v>505353,76</v>
+        <v>505353.76</v>
       </c>
       <c r="F141" t="str">
         <f t="shared" si="31"/>
-        <v>0042803,27</v>
+        <v>0042803.27</v>
       </c>
       <c r="G141">
         <f t="shared" si="27"/>
@@ -10438,7 +10480,7 @@
         <v>4.4675749999999992</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>402</v>
       </c>
@@ -10453,11 +10495,11 @@
       </c>
       <c r="E142" t="str">
         <f t="shared" si="30"/>
-        <v>505355,36</v>
+        <v>505355.36</v>
       </c>
       <c r="F142" t="str">
         <f t="shared" si="31"/>
-        <v xml:space="preserve">0042804,51 </v>
+        <v xml:space="preserve">0042804.51 </v>
       </c>
       <c r="G142">
         <f t="shared" si="27"/>
@@ -10492,7 +10534,7 @@
         <v>4.467919444444445</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>402</v>
       </c>
@@ -10507,11 +10549,11 @@
       </c>
       <c r="E143" t="str">
         <f t="shared" si="30"/>
-        <v>505353,89</v>
+        <v>505353.89</v>
       </c>
       <c r="F143" t="str">
         <f t="shared" si="31"/>
-        <v>0042804,37</v>
+        <v>0042804.37</v>
       </c>
       <c r="G143">
         <f t="shared" si="27"/>
@@ -10546,7 +10588,7 @@
         <v>4.4678805555555563</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>402</v>
       </c>
@@ -10561,11 +10603,11 @@
       </c>
       <c r="E144" t="str">
         <f t="shared" si="30"/>
-        <v>505355,82</v>
+        <v>505355.82</v>
       </c>
       <c r="F144" t="str">
         <f t="shared" si="31"/>
-        <v>0042805,36</v>
+        <v>0042805.36</v>
       </c>
       <c r="G144">
         <f t="shared" si="27"/>
@@ -10600,7 +10642,7 @@
         <v>4.4681555555555557</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>402</v>
       </c>
@@ -10615,11 +10657,11 @@
       </c>
       <c r="E145" t="str">
         <f t="shared" si="30"/>
-        <v>505354,46</v>
+        <v>505354.46</v>
       </c>
       <c r="F145" t="str">
         <f t="shared" si="31"/>
-        <v>0042806,35</v>
+        <v>0042806.35</v>
       </c>
       <c r="G145">
         <f t="shared" si="27"/>
@@ -10654,7 +10696,7 @@
         <v>4.468430555555555</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>402</v>
       </c>
@@ -10669,11 +10711,11 @@
       </c>
       <c r="E146" t="str">
         <f t="shared" si="30"/>
-        <v>505356,39</v>
+        <v>505356.39</v>
       </c>
       <c r="F146" t="str">
         <f t="shared" si="31"/>
-        <v>0042807,35</v>
+        <v>0042807.35</v>
       </c>
       <c r="G146">
         <f t="shared" si="27"/>
@@ -10708,7 +10750,7 @@
         <v>4.4687083333333328</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>402</v>
       </c>
@@ -10723,11 +10765,11 @@
       </c>
       <c r="E147" t="str">
         <f t="shared" si="30"/>
-        <v>505354,90</v>
+        <v>505354.90</v>
       </c>
       <c r="F147" t="str">
         <f t="shared" si="31"/>
-        <v>0042807,23</v>
+        <v>0042807.23</v>
       </c>
       <c r="G147">
         <f t="shared" si="27"/>
@@ -10762,7 +10804,7 @@
         <v>4.4686750000000011</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>402</v>
       </c>
@@ -10777,11 +10819,11 @@
       </c>
       <c r="E148" t="str">
         <f t="shared" si="30"/>
-        <v>505356,50</v>
+        <v>505356.50</v>
       </c>
       <c r="F148" t="str">
         <f t="shared" si="31"/>
-        <v>0042808,46</v>
+        <v>0042808.46</v>
       </c>
       <c r="G148">
         <f t="shared" si="27"/>
@@ -10816,7 +10858,7 @@
         <v>4.4690166666666666</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>402</v>
       </c>
@@ -10831,11 +10873,11 @@
       </c>
       <c r="E149" t="str">
         <f t="shared" si="30"/>
-        <v>505355,04</v>
+        <v>505355.04</v>
       </c>
       <c r="F149" t="str">
         <f t="shared" si="31"/>
-        <v>0042808,33</v>
+        <v>0042808.33</v>
       </c>
       <c r="G149">
         <f t="shared" si="27"/>
@@ -10870,7 +10912,7 @@
         <v>4.4689805555555564</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>402</v>
       </c>
@@ -10885,11 +10927,11 @@
       </c>
       <c r="E150" t="str">
         <f t="shared" si="30"/>
-        <v>505356,96</v>
+        <v>505356.96</v>
       </c>
       <c r="F150" t="str">
         <f t="shared" si="31"/>
-        <v>0042809,32</v>
+        <v>0042809.32</v>
       </c>
       <c r="G150">
         <f t="shared" si="27"/>
@@ -10924,7 +10966,7 @@
         <v>4.4692555555555558</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>402</v>
       </c>
@@ -10939,11 +10981,11 @@
       </c>
       <c r="E151" t="str">
         <f t="shared" si="30"/>
-        <v>505355,61</v>
+        <v>505355.61</v>
       </c>
       <c r="F151" t="str">
         <f t="shared" si="31"/>
-        <v>0042810,30</v>
+        <v>0042810.30</v>
       </c>
       <c r="G151">
         <f t="shared" si="27"/>
@@ -10978,7 +11020,7 @@
         <v>4.4695277777777784</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>402</v>
       </c>
@@ -10993,11 +11035,11 @@
       </c>
       <c r="E152" t="str">
         <f t="shared" si="30"/>
-        <v>505357,53</v>
+        <v>505357.53</v>
       </c>
       <c r="F152" t="str">
         <f t="shared" si="31"/>
-        <v>0042811,30</v>
+        <v>0042811.30</v>
       </c>
       <c r="G152">
         <f t="shared" si="27"/>
@@ -11032,7 +11074,7 @@
         <v>4.4698055555555563</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>402</v>
       </c>
@@ -11047,11 +11089,11 @@
       </c>
       <c r="E153" t="str">
         <f t="shared" si="30"/>
-        <v>505356,04</v>
+        <v>505356.04</v>
       </c>
       <c r="F153" t="str">
         <f t="shared" si="31"/>
-        <v>0042811,18</v>
+        <v>0042811.18</v>
       </c>
       <c r="G153">
         <f t="shared" si="27"/>
@@ -11086,7 +11128,7 @@
         <v>4.4697722222222227</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>402</v>
       </c>
@@ -11101,11 +11143,11 @@
       </c>
       <c r="E154" t="str">
         <f t="shared" si="30"/>
-        <v>505357,67</v>
+        <v>505357.67</v>
       </c>
       <c r="F154" t="str">
         <f t="shared" si="31"/>
-        <v>0042812,40</v>
+        <v>0042812.40</v>
       </c>
       <c r="G154">
         <f t="shared" si="27"/>
@@ -11140,7 +11182,7 @@
         <v>4.4701111111111116</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>402</v>
       </c>
@@ -11155,11 +11197,11 @@
       </c>
       <c r="E155" t="str">
         <f t="shared" si="30"/>
-        <v>505356,18</v>
+        <v>505356.18</v>
       </c>
       <c r="F155" t="str">
         <f t="shared" si="31"/>
-        <v>0042812,28</v>
+        <v>0042812.28</v>
       </c>
       <c r="G155">
         <f t="shared" si="27"/>
@@ -11194,7 +11236,7 @@
         <v>4.4700777777777772</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>402</v>
       </c>
@@ -11209,11 +11251,11 @@
       </c>
       <c r="E156" t="str">
         <f t="shared" si="30"/>
-        <v>505358,11</v>
+        <v>505358.11</v>
       </c>
       <c r="F156" t="str">
         <f t="shared" si="31"/>
-        <v>0042813,27</v>
+        <v>0042813.27</v>
       </c>
       <c r="G156">
         <f t="shared" si="27"/>
@@ -11248,7 +11290,7 @@
         <v>4.4703527777777774</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>402</v>
       </c>
@@ -11263,11 +11305,11 @@
       </c>
       <c r="E157" t="str">
         <f t="shared" si="30"/>
-        <v>505356,43</v>
+        <v>505356.43</v>
       </c>
       <c r="F157" t="str">
         <f t="shared" si="31"/>
-        <v>0042814,49</v>
+        <v>0042814.49</v>
       </c>
       <c r="G157">
         <f t="shared" si="27"/>
@@ -11302,7 +11344,7 @@
         <v>4.4706916666666663</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>399</v>
       </c>
@@ -11317,11 +11359,11 @@
       </c>
       <c r="E158" t="str">
         <f t="shared" si="30"/>
-        <v>505403,08</v>
+        <v>505403.08</v>
       </c>
       <c r="F158" t="str">
         <f t="shared" si="31"/>
-        <v>0042702,77</v>
+        <v>0042702.77</v>
       </c>
       <c r="G158">
         <f t="shared" si="27"/>
@@ -11356,7 +11398,7 @@
         <v>4.4507694444444441</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>399</v>
       </c>
@@ -11371,11 +11413,11 @@
       </c>
       <c r="E159" t="str">
         <f t="shared" si="30"/>
-        <v>505403,88</v>
+        <v>505403.88</v>
       </c>
       <c r="F159" t="str">
         <f t="shared" si="31"/>
-        <v>0042703,42</v>
+        <v>0042703.42</v>
       </c>
       <c r="G159">
         <f t="shared" si="27"/>
@@ -11410,7 +11452,7 @@
         <v>4.4509499999999997</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>399</v>
       </c>
@@ -11425,11 +11467,11 @@
       </c>
       <c r="E160" t="str">
         <f t="shared" si="30"/>
-        <v>505403,67</v>
+        <v>505403.67</v>
       </c>
       <c r="F160" t="str">
         <f t="shared" si="31"/>
-        <v>0042704,82</v>
+        <v>0042704.82</v>
       </c>
       <c r="G160">
         <f t="shared" si="27"/>
@@ -11464,7 +11506,7 @@
         <v>4.4513388888888894</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>399</v>
       </c>
@@ -11479,11 +11521,11 @@
       </c>
       <c r="E161" t="str">
         <f t="shared" si="30"/>
-        <v>505404,30</v>
+        <v>505404.30</v>
       </c>
       <c r="F161" t="str">
         <f t="shared" si="31"/>
-        <v>0042707,00</v>
+        <v>0042707.00</v>
       </c>
       <c r="G161">
         <f t="shared" si="27"/>
@@ -11518,7 +11560,7 @@
         <v>4.4519444444444449</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>399</v>
       </c>
@@ -11533,11 +11575,11 @@
       </c>
       <c r="E162" t="str">
         <f t="shared" si="30"/>
-        <v>505405,10</v>
+        <v>505405.10</v>
       </c>
       <c r="F162" t="str">
         <f t="shared" si="31"/>
-        <v>0042707,65</v>
+        <v>0042707.65</v>
       </c>
       <c r="G162">
         <f t="shared" ref="G162:G177" si="37">_xlfn.FLOOR.MATH(E162/10000)</f>
@@ -11572,7 +11614,7 @@
         <v>4.4521250000000006</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>399</v>
       </c>
@@ -11587,11 +11629,11 @@
       </c>
       <c r="E163" t="str">
         <f t="shared" si="30"/>
-        <v>505404,89</v>
+        <v>505404.89</v>
       </c>
       <c r="F163" t="str">
         <f t="shared" si="31"/>
-        <v>0042709,05</v>
+        <v>0042709.05</v>
       </c>
       <c r="G163">
         <f t="shared" si="37"/>
@@ -11626,7 +11668,7 @@
         <v>4.4525138888888902</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>399</v>
       </c>
@@ -11641,11 +11683,11 @@
       </c>
       <c r="E164" t="str">
         <f t="shared" si="30"/>
-        <v>505407,35</v>
+        <v>505407.35</v>
       </c>
       <c r="F164" t="str">
         <f t="shared" si="31"/>
-        <v>0042715,01</v>
+        <v>0042715.01</v>
       </c>
       <c r="G164">
         <f t="shared" si="37"/>
@@ -11680,7 +11722,7 @@
         <v>4.4541694444444451</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>399</v>
       </c>
@@ -11695,11 +11737,11 @@
       </c>
       <c r="E165" t="str">
         <f t="shared" si="30"/>
-        <v>505409,02</v>
+        <v>505409.02</v>
       </c>
       <c r="F165" t="str">
         <f t="shared" si="31"/>
-        <v>0042720,78</v>
+        <v>0042720.78</v>
       </c>
       <c r="G165">
         <f t="shared" si="37"/>
@@ -11734,7 +11776,7 @@
         <v>4.4557722222222225</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>399</v>
       </c>
@@ -11749,11 +11791,11 @@
       </c>
       <c r="E166" t="str">
         <f t="shared" si="30"/>
-        <v>505409,50</v>
+        <v>505409.50</v>
       </c>
       <c r="F166" t="str">
         <f t="shared" si="31"/>
-        <v>0042723,92</v>
+        <v>0042723.92</v>
       </c>
       <c r="G166">
         <f t="shared" si="37"/>
@@ -11788,7 +11830,7 @@
         <v>4.4566444444444437</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>399</v>
       </c>
@@ -11803,11 +11845,11 @@
       </c>
       <c r="E167" t="str">
         <f t="shared" si="30"/>
-        <v>505410,68</v>
+        <v>505410.68</v>
       </c>
       <c r="F167" t="str">
         <f t="shared" si="31"/>
-        <v>0042726,55</v>
+        <v>0042726.55</v>
       </c>
       <c r="G167">
         <f t="shared" si="37"/>
@@ -11842,7 +11884,7 @@
         <v>4.4573750000000008</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>399</v>
       </c>
@@ -11857,11 +11899,11 @@
       </c>
       <c r="E168" t="str">
         <f t="shared" si="30"/>
-        <v>505411,17</v>
+        <v>505411.17</v>
       </c>
       <c r="F168" t="str">
         <f t="shared" si="31"/>
-        <v>0042729,69</v>
+        <v>0042729.69</v>
       </c>
       <c r="G168">
         <f t="shared" si="37"/>
@@ -11896,7 +11938,7 @@
         <v>4.4582472222222229</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>399</v>
       </c>
@@ -11911,11 +11953,11 @@
       </c>
       <c r="E169" t="str">
         <f t="shared" si="30"/>
-        <v>505412,35</v>
+        <v>505412.35</v>
       </c>
       <c r="F169" t="str">
         <f t="shared" si="31"/>
-        <v>0042732,32</v>
+        <v>0042732.32</v>
       </c>
       <c r="G169">
         <f t="shared" si="37"/>
@@ -11950,7 +11992,7 @@
         <v>4.4589777777777782</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>399</v>
       </c>
@@ -11965,11 +12007,11 @@
       </c>
       <c r="E170" t="str">
         <f t="shared" si="30"/>
-        <v>505412,84</v>
+        <v>505412.84</v>
       </c>
       <c r="F170" t="str">
         <f t="shared" si="31"/>
-        <v>0042735,46</v>
+        <v>0042735.46</v>
       </c>
       <c r="G170">
         <f t="shared" si="37"/>
@@ -12004,7 +12046,7 @@
         <v>4.4598500000000003</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>399</v>
       </c>
@@ -12019,11 +12061,11 @@
       </c>
       <c r="E171" t="str">
         <f t="shared" si="30"/>
-        <v>505414,02</v>
+        <v>505414.02</v>
       </c>
       <c r="F171" t="str">
         <f t="shared" si="31"/>
-        <v>0042738,10</v>
+        <v>0042738.10</v>
       </c>
       <c r="G171">
         <f t="shared" si="37"/>
@@ -12058,7 +12100,7 @@
         <v>4.4605833333333331</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>399</v>
       </c>
@@ -12073,11 +12115,11 @@
       </c>
       <c r="E172" t="str">
         <f t="shared" si="30"/>
-        <v xml:space="preserve">505414,51 </v>
+        <v xml:space="preserve">505414.51 </v>
       </c>
       <c r="F172" t="str">
         <f t="shared" si="31"/>
-        <v xml:space="preserve">0042741,24 </v>
+        <v xml:space="preserve">0042741.24 </v>
       </c>
       <c r="G172">
         <f t="shared" si="37"/>
@@ -12112,7 +12154,7 @@
         <v>4.4614555555555553</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>399</v>
       </c>
@@ -12127,11 +12169,11 @@
       </c>
       <c r="E173" t="str">
         <f t="shared" si="30"/>
-        <v xml:space="preserve">505415,66 </v>
+        <v xml:space="preserve">505415.66 </v>
       </c>
       <c r="F173" t="str">
         <f t="shared" si="31"/>
-        <v xml:space="preserve">0042744,22 </v>
+        <v xml:space="preserve">0042744.22 </v>
       </c>
       <c r="G173">
         <f t="shared" si="37"/>
@@ -12166,7 +12208,7 @@
         <v>4.4622833333333336</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>399</v>
       </c>
@@ -12181,11 +12223,11 @@
       </c>
       <c r="E174" t="str">
         <f t="shared" si="30"/>
-        <v xml:space="preserve">505416,07 </v>
+        <v xml:space="preserve">505416.07 </v>
       </c>
       <c r="F174" t="str">
         <f t="shared" si="31"/>
-        <v xml:space="preserve">0042747,27 </v>
+        <v xml:space="preserve">0042747.27 </v>
       </c>
       <c r="G174">
         <f t="shared" si="37"/>
@@ -12220,7 +12262,7 @@
         <v>4.4631305555555549</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>399</v>
       </c>
@@ -12235,11 +12277,11 @@
       </c>
       <c r="E175" t="str">
         <f t="shared" si="30"/>
-        <v xml:space="preserve">505416,89 </v>
+        <v xml:space="preserve">505416.89 </v>
       </c>
       <c r="F175" t="str">
         <f t="shared" si="31"/>
-        <v xml:space="preserve">0042748,48 </v>
+        <v xml:space="preserve">0042748.48 </v>
       </c>
       <c r="G175">
         <f t="shared" si="37"/>
@@ -12274,7 +12316,7 @@
         <v>4.463466666666668</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>399</v>
       </c>
@@ -12289,11 +12331,11 @@
       </c>
       <c r="E176" t="str">
         <f t="shared" si="30"/>
-        <v xml:space="preserve">505416,87 </v>
+        <v xml:space="preserve">505416.87 </v>
       </c>
       <c r="F176" t="str">
         <f t="shared" si="31"/>
-        <v xml:space="preserve">0042750,03 </v>
+        <v xml:space="preserve">0042750.03 </v>
       </c>
       <c r="G176">
         <f t="shared" si="37"/>
@@ -12328,7 +12370,7 @@
         <v>4.4638972222222222</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="15" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>399</v>
       </c>
@@ -12343,11 +12385,11 @@
       </c>
       <c r="E177" t="str">
         <f t="shared" si="30"/>
-        <v>505416,92</v>
+        <v>505416.92</v>
       </c>
       <c r="F177" t="str">
         <f t="shared" si="31"/>
-        <v xml:space="preserve">0042753,41 </v>
+        <v xml:space="preserve">0042753.41 </v>
       </c>
       <c r="G177">
         <f t="shared" si="37"/>
@@ -12382,12 +12424,12 @@
         <v>4.4648361111111123</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="J178">
         <v>50.914810202894301</v>
@@ -12396,12 +12438,12 @@
         <v>4.4967164240292599</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>404</v>
+        <v>409</v>
       </c>
       <c r="J179">
         <v>50.914594964808401</v>
@@ -12410,12 +12452,12 @@
         <v>4.4961626144487203</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="J180">
         <v>50.914417990525401</v>
@@ -12424,12 +12466,12 @@
         <v>4.4956467370312296</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="J181">
         <v>50.913988691865498</v>
@@ -12438,12 +12480,12 @@
         <v>4.49443353948016</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="J182">
         <v>50.913738412749403</v>
@@ -12452,12 +12494,12 @@
         <v>4.4937839670262703</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
+        <v>407</v>
+      </c>
+      <c r="B183" s="2" t="s">
         <v>413</v>
-      </c>
-      <c r="B183" s="2" t="s">
-        <v>408</v>
       </c>
       <c r="J183">
         <v>50.913510885112302</v>
@@ -12466,12 +12508,12 @@
         <v>4.49312537273273</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="J184">
         <v>50.913101332544898</v>
@@ -12480,12 +12522,12 @@
         <v>4.4911946990088802</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="J185">
         <v>50.913010320377801</v>
@@ -12494,12 +12536,12 @@
         <v>4.4905721920739001</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="J186">
         <v>50.912703152999498</v>
@@ -12508,18 +12550,158 @@
         <v>4.4899226196199997</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="J187">
         <v>50.912526815255298</v>
       </c>
       <c r="N187">
         <v>4.4894354402795802</v>
+      </c>
+    </row>
+    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>424</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="J188">
+        <v>50.896245766464403</v>
+      </c>
+      <c r="N188">
+        <v>4.4672248103730601</v>
+      </c>
+    </row>
+    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>424</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="J189">
+        <v>50.8963837586831</v>
+      </c>
+      <c r="N189">
+        <v>4.46778502646987</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>424</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="J190">
+        <v>50.895469514396801</v>
+      </c>
+      <c r="N190">
+        <v>4.4665204829185798</v>
+      </c>
+    </row>
+    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>424</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="J191">
+        <v>50.895766480337898</v>
+      </c>
+      <c r="N191">
+        <v>4.4679075168651199</v>
+      </c>
+    </row>
+    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>424</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="J192">
+        <v>50.895932323109399</v>
+      </c>
+      <c r="N192">
+        <v>4.4684262655108098</v>
+      </c>
+    </row>
+    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>424</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="J193">
+        <v>50.897002698050599</v>
+      </c>
+      <c r="N193">
+        <v>4.4646363213440097</v>
+      </c>
+    </row>
+    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>424</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="J194">
+        <v>50.8971752854549</v>
+      </c>
+      <c r="N194">
+        <v>4.4652878767248501</v>
+      </c>
+    </row>
+    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>424</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="J195">
+        <v>50.897315816901099</v>
+      </c>
+      <c r="N195">
+        <v>4.46589393550867</v>
+      </c>
+    </row>
+    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>424</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="J196">
+        <v>50.8974619486347</v>
+      </c>
+      <c r="N196">
+        <v>4.4664137570469196</v>
+      </c>
+    </row>
+    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>424</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="J197">
+        <v>50.897637972154797</v>
+      </c>
+      <c r="N197">
+        <v>4.4670373493481401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>